<commit_message>
Add missing label for R41 in the BOM
</commit_message>
<xml_diff>
--- a/reference/hardware/v0.3/v0.3.1_bom.xlsx
+++ b/reference/hardware/v0.3/v0.3.1_bom.xlsx
@@ -1,21 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="25808"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/josh/Documents/Arduino/speeduino/speeduino/reference/hardware/v0.3/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16760" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Full Kit" sheetId="1" r:id="rId1"/>
     <sheet name="2 Channel" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -359,9 +354,6 @@
     <t>Total of Materials:Cost to Manufacture</t>
   </si>
   <si>
-    <t>R2,4,6,8,22,</t>
-  </si>
-  <si>
     <t>R1,3</t>
   </si>
   <si>
@@ -717,6 +709,9 @@
   </si>
   <si>
     <t>399-4206-ND</t>
+  </si>
+  <si>
+    <t>R2,4,6,8,22,41</t>
   </si>
 </sst>
 </file>
@@ -1421,11 +1416,11 @@
   </sheetPr>
   <dimension ref="A1:O52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="18.83203125" style="20" customWidth="1"/>
     <col min="2" max="2" width="46.6640625" customWidth="1"/>
@@ -1438,12 +1433,12 @@
     <col min="15" max="15" width="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="17" thickBot="1">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -1455,7 +1450,7 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>4</v>
@@ -1479,13 +1474,13 @@
         <v>10</v>
       </c>
       <c r="N1" s="23" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="O1" s="23" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="17" thickBot="1">
       <c r="A2" s="18"/>
       <c r="B2" s="4"/>
       <c r="C2" s="3"/>
@@ -1508,19 +1503,19 @@
         <v xml:space="preserve">x </v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" ht="17" thickBot="1">
       <c r="A3" s="21">
         <f>LEN(B3)-LEN(SUBSTITUTE(B3,",",""))+1</f>
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>12</v>
@@ -1533,10 +1528,10 @@
         <v>16</v>
       </c>
       <c r="I3" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="J3" s="2" t="s">
         <v>197</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>198</v>
       </c>
       <c r="K3" s="5">
         <v>1.7</v>
@@ -1555,19 +1550,19 @@
         <v>Capacitor - 1x 10uF</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" ht="17" thickBot="1">
       <c r="A4" s="21">
         <f>LEN(B4)-LEN(SUBSTITUTE(B4,",",""))+1</f>
         <v>5</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>15</v>
@@ -1580,10 +1575,10 @@
         <v>16</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="K4" s="5">
         <v>0.66</v>
@@ -1602,19 +1597,19 @@
         <v>Capacitor - 5x 0.22uF</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" ht="27" thickBot="1">
       <c r="A5" s="21">
         <f>LEN(B5)-LEN(SUBSTITUTE(B5,",",""))+1</f>
         <v>7</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>17</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>15</v>
@@ -1627,10 +1622,10 @@
         <v>16</v>
       </c>
       <c r="I5" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="J5" s="2" t="s">
         <v>191</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>192</v>
       </c>
       <c r="K5" s="5">
         <v>0.32</v>
@@ -1649,19 +1644,19 @@
         <v>Capacitor - 7x 0.1uF / 100nF</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" ht="17" thickBot="1">
       <c r="A6" s="21">
         <f>LEN(B6)-LEN(SUBSTITUTE(B6,",",""))+1</f>
         <v>1</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>18</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>12</v>
@@ -1674,10 +1669,10 @@
         <v>16</v>
       </c>
       <c r="I6" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="J6" s="2" t="s">
         <v>200</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>201</v>
       </c>
       <c r="K6" s="5">
         <v>1.57</v>
@@ -1696,19 +1691,19 @@
         <v>Capacitor - 1x 47uF</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" ht="27" thickBot="1">
       <c r="A7" s="21">
         <f t="shared" ref="A7:A9" si="3">LEN(B7)-LEN(SUBSTITUTE(B7,",",""))+1</f>
         <v>1</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>15</v>
@@ -1721,10 +1716,10 @@
         <v>13</v>
       </c>
       <c r="I7" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="J7" s="2" t="s">
         <v>202</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>203</v>
       </c>
       <c r="K7" s="5">
         <v>0.62</v>
@@ -1743,19 +1738,19 @@
         <v>Capacitor - 1x 0.33uF</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" ht="17" thickBot="1">
       <c r="A8" s="21">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>20</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>15</v>
@@ -1768,10 +1763,10 @@
         <v>16</v>
       </c>
       <c r="I8" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="J8" s="2" t="s">
         <v>206</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>207</v>
       </c>
       <c r="K8" s="5">
         <v>0.24</v>
@@ -1790,19 +1785,19 @@
         <v>Capacitor - 1x 0.01uF</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" ht="17" thickBot="1">
       <c r="A9" s="21">
         <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>21</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>15</v>
@@ -1815,10 +1810,10 @@
         <v>16</v>
       </c>
       <c r="I9" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="J9" s="2" t="s">
         <v>188</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>189</v>
       </c>
       <c r="K9" s="5">
         <v>0.66</v>
@@ -1837,19 +1832,19 @@
         <v>Capacitor - 3x 1uF</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" ht="17" thickBot="1">
       <c r="A10" s="21">
         <f>LEN(B10)-LEN(SUBSTITUTE(B10,",",""))+1</f>
         <v>1</v>
       </c>
       <c r="B10" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>151</v>
-      </c>
       <c r="D10" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>15</v>
@@ -1860,10 +1855,10 @@
         <v>16</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K10" s="5">
         <v>0.25</v>
@@ -1882,7 +1877,7 @@
         <v>Capacitor - 1x 4.7nF</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" ht="17" thickBot="1">
       <c r="A11" s="18"/>
       <c r="B11" s="4"/>
       <c r="C11" s="3"/>
@@ -1901,7 +1896,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" ht="17" thickBot="1">
       <c r="A12" s="18"/>
       <c r="B12" s="4"/>
       <c r="C12" s="3"/>
@@ -1920,16 +1915,16 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="40" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" ht="40" thickBot="1">
       <c r="A13" s="21">
         <f>LEN(B13)-LEN(SUBSTITUTE(B13,",",""))+1</f>
         <v>1</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D13" s="7" t="s">
         <v>22</v>
@@ -1967,16 +1962,16 @@
         <v>Diode - 1x 1N5919BG Zener</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="40" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" ht="40" thickBot="1">
       <c r="A14" s="21">
         <f>LEN(B14)-LEN(SUBSTITUTE(B14,",",""))+1</f>
         <v>12</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>28</v>
@@ -2014,29 +2009,29 @@
         <v>Diode - 12x 1N5818-TP Schottky</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" ht="17" thickBot="1">
       <c r="A15" s="21">
         <f>LEN(B15)-LEN(SUBSTITUTE(B15,",",""))+1</f>
         <v>8</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>31</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
       <c r="J15" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K15" s="5">
         <v>0.47</v>
@@ -2055,13 +2050,13 @@
         <v>Diode - 8x LED-Red</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="40" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" ht="40" thickBot="1">
       <c r="A16" s="21">
         <f>LEN(B16)-LEN(SUBSTITUTE(B16,",",""))+1</f>
         <v>4</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>32</v>
@@ -2102,7 +2097,7 @@
         <v>Diode - 4x 1N4004</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" ht="17" thickBot="1">
       <c r="A17" s="18"/>
       <c r="B17" s="4"/>
       <c r="C17" s="3"/>
@@ -2125,7 +2120,7 @@
         <v xml:space="preserve">x </v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" ht="17" thickBot="1">
       <c r="A18" s="19"/>
       <c r="B18" s="4"/>
       <c r="C18" s="3"/>
@@ -2148,7 +2143,7 @@
         <v xml:space="preserve">x </v>
       </c>
     </row>
-    <row r="19" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" ht="17" thickBot="1">
       <c r="A19" s="18"/>
       <c r="B19" s="4"/>
       <c r="C19" s="3"/>
@@ -2171,12 +2166,12 @@
         <v xml:space="preserve">x </v>
       </c>
     </row>
-    <row r="20" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" ht="27" thickBot="1">
       <c r="A20" s="21">
         <v>1</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>36</v>
@@ -2217,7 +2212,7 @@
         <v>1x Surge Protection</v>
       </c>
     </row>
-    <row r="21" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" ht="17" thickBot="1">
       <c r="A21" s="18"/>
       <c r="B21" s="4"/>
       <c r="C21" s="3"/>
@@ -2240,30 +2235,30 @@
         <v xml:space="preserve">x </v>
       </c>
     </row>
-    <row r="22" spans="1:15" ht="40" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" ht="40" thickBot="1">
       <c r="A22" s="21">
         <v>14</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
       <c r="H22" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="K22" s="3">
         <v>0.40200000000000002</v>
@@ -2273,7 +2268,7 @@
         <v>5.6280000000000001</v>
       </c>
       <c r="M22" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="N22" s="4" t="str">
         <f t="shared" si="1"/>
@@ -2284,18 +2279,18 @@
         <v>14x Dual Terminal Block</v>
       </c>
     </row>
-    <row r="23" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" ht="17" thickBot="1">
       <c r="A23" s="21">
         <v>5</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>42</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
@@ -2303,7 +2298,7 @@
       <c r="H23" s="3"/>
       <c r="I23" s="3"/>
       <c r="J23" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="K23" s="5">
         <v>0.1</v>
@@ -2322,18 +2317,18 @@
         <v>5x Jumper</v>
       </c>
     </row>
-    <row r="24" spans="1:15" ht="40" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" ht="40" thickBot="1">
       <c r="A24" s="21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
@@ -2341,32 +2336,32 @@
         <v>1</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="K24" s="6">
         <v>0.56000000000000005</v>
       </c>
       <c r="L24" s="6">
         <f>K24*A24</f>
-        <v>0.56000000000000005</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="M24" s="4"/>
       <c r="N24" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>1,S1012EC-40-ND</v>
+        <v>2,S1012EC-40-ND</v>
       </c>
       <c r="O24" t="str">
         <f t="shared" si="5"/>
-        <v>1x 40 POS 0.100 Pin Header</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+        <v>2x 40 POS 0.100 Pin Header</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" ht="17" thickBot="1">
       <c r="A25" s="18"/>
       <c r="B25" s="4"/>
       <c r="C25" s="3"/>
@@ -2389,7 +2384,7 @@
         <v xml:space="preserve">x </v>
       </c>
     </row>
-    <row r="26" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" ht="17" thickBot="1">
       <c r="A26" s="18"/>
       <c r="B26" s="4"/>
       <c r="C26" s="3"/>
@@ -2412,19 +2407,19 @@
         <v xml:space="preserve">x </v>
       </c>
     </row>
-    <row r="27" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" ht="27" thickBot="1">
       <c r="A27" s="21">
         <f>LEN(B27)-LEN(SUBSTITUTE(B27,",",""))+1</f>
         <v>8</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>79</v>
@@ -2437,10 +2432,10 @@
         <v>43</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="K27" s="6">
         <v>1.51</v>
@@ -2459,7 +2454,7 @@
         <v>8x 62A MOSFET N-CH</v>
       </c>
     </row>
-    <row r="28" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" ht="17" thickBot="1">
       <c r="A28" s="18"/>
       <c r="B28" s="4"/>
       <c r="C28" s="3"/>
@@ -2478,7 +2473,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" ht="17" thickBot="1">
       <c r="A29" s="18"/>
       <c r="B29" s="4"/>
       <c r="C29" s="3"/>
@@ -2497,13 +2492,13 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" ht="17" thickBot="1">
       <c r="A30" s="21">
         <f>LEN(B30)-LEN(SUBSTITUTE(B30,",",""))+1</f>
         <v>5</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>44</v>
@@ -2542,13 +2537,13 @@
         <v>Resistor - 5x 10k</v>
       </c>
     </row>
-    <row r="31" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" ht="17" thickBot="1">
       <c r="A31" s="21">
         <f>LEN(B31)-LEN(SUBSTITUTE(B31,",",""))+1</f>
         <v>12</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>49</v>
@@ -2587,29 +2582,29 @@
         <v>Resistor - 12x 1k</v>
       </c>
     </row>
-    <row r="32" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" ht="27" thickBot="1">
       <c r="A32" s="21">
         <f>LEN(B32)-LEN(SUBSTITUTE(B32,",",""))+1</f>
         <v>8</v>
       </c>
       <c r="B32" s="13" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C32" s="14">
         <v>680</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E32" s="3"/>
       <c r="F32" s="14"/>
       <c r="G32" s="14"/>
       <c r="H32" s="14" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="I32" s="7"/>
       <c r="J32" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="K32" s="15">
         <v>0.22</v>
@@ -2619,7 +2614,7 @@
         <v>1.76</v>
       </c>
       <c r="M32" s="13" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="N32" s="4" t="str">
         <f t="shared" si="1"/>
@@ -2630,13 +2625,13 @@
         <v>Resistor - 8x 680</v>
       </c>
     </row>
-    <row r="33" spans="1:15" ht="40" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" ht="40" thickBot="1">
       <c r="A33" s="21">
         <f>LEN(B33)-LEN(SUBSTITUTE(B33,",",""))+1</f>
         <v>6</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>88</v>
+        <v>207</v>
       </c>
       <c r="C33" s="3">
         <v>470</v>
@@ -2675,15 +2670,15 @@
         <v>Resistor - 6x 470</v>
       </c>
     </row>
-    <row r="34" spans="1:15" ht="40" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" ht="40" thickBot="1">
       <c r="A34" s="21">
         <v>2</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D34" s="3" t="s">
         <v>57</v>
@@ -2721,15 +2716,15 @@
         <v>Resistor - 2x 0.1% 2.49k</v>
       </c>
     </row>
-    <row r="35" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" ht="17" thickBot="1">
       <c r="A35" s="21">
         <v>1</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D35" s="3" t="s">
         <v>62</v>
@@ -2756,7 +2751,7 @@
         <v>0.46</v>
       </c>
       <c r="M35" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="N35" s="4" t="str">
         <f t="shared" si="1"/>
@@ -2767,15 +2762,15 @@
         <v>Resistor - 1x 0.1% 3.9k</v>
       </c>
     </row>
-    <row r="36" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" ht="17" thickBot="1">
       <c r="A36" s="21">
         <v>1</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D36" s="3" t="s">
         <v>65</v>
@@ -2802,7 +2797,7 @@
         <v>0.46</v>
       </c>
       <c r="M36" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="N36" s="4" t="str">
         <f t="shared" si="1"/>
@@ -2813,13 +2808,13 @@
         <v>Resistor - 1x 0.1% 1.0k</v>
       </c>
     </row>
-    <row r="37" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" ht="17" thickBot="1">
       <c r="A37" s="21">
         <f t="shared" ref="A37:A38" si="8">LEN(B37)-LEN(SUBSTITUTE(B37,",",""))+1</f>
         <v>12</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C37" s="3" t="s">
         <v>68</v>
@@ -2858,13 +2853,13 @@
         <v>Resistor - 12x 100k</v>
       </c>
     </row>
-    <row r="38" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" ht="17" thickBot="1">
       <c r="A38" s="21">
         <f t="shared" si="8"/>
         <v>4</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C38" s="3">
         <v>160</v>
@@ -2903,7 +2898,7 @@
         <v>Resistor - 4x 160</v>
       </c>
     </row>
-    <row r="39" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" ht="17" thickBot="1">
       <c r="A39" s="18"/>
       <c r="B39" s="4"/>
       <c r="C39" s="3"/>
@@ -2922,7 +2917,7 @@
         <v/>
       </c>
     </row>
-    <row r="40" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" ht="17" thickBot="1">
       <c r="A40" s="18"/>
       <c r="B40" s="4"/>
       <c r="C40" s="3"/>
@@ -2941,7 +2936,7 @@
         <v/>
       </c>
     </row>
-    <row r="41" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" ht="27" thickBot="1">
       <c r="A41" s="21">
         <v>1</v>
       </c>
@@ -2987,21 +2982,21 @@
         <v>1x LM2940T-5.0/NOPB</v>
       </c>
     </row>
-    <row r="42" spans="1:15" ht="40" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15" ht="40" thickBot="1">
       <c r="A42" s="21">
         <v>1</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F42" s="3"/>
       <c r="G42" s="3">
@@ -3012,7 +3007,7 @@
       </c>
       <c r="I42" s="3"/>
       <c r="J42" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K42" s="6">
         <v>15.41</v>
@@ -3031,21 +3026,21 @@
         <v>1x 1-Bar MAP sensor</v>
       </c>
     </row>
-    <row r="43" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" ht="27" thickBot="1">
       <c r="A43" s="24">
         <v>2</v>
       </c>
       <c r="B43" s="13" t="s">
+        <v>168</v>
+      </c>
+      <c r="C43" s="14" t="s">
         <v>169</v>
       </c>
-      <c r="C43" s="14" t="s">
+      <c r="D43" s="7" t="s">
         <v>170</v>
       </c>
-      <c r="D43" s="7" t="s">
+      <c r="E43" s="3" t="s">
         <v>171</v>
-      </c>
-      <c r="E43" s="3" t="s">
-        <v>172</v>
       </c>
       <c r="F43" s="14"/>
       <c r="G43" s="14">
@@ -3056,7 +3051,7 @@
       </c>
       <c r="I43" s="14"/>
       <c r="J43" s="14" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="K43" s="25">
         <v>2.92</v>
@@ -3075,21 +3070,21 @@
         <v>2x TC4424EPA</v>
       </c>
     </row>
-    <row r="44" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" ht="27" thickBot="1">
       <c r="A44" s="21">
         <v>1</v>
       </c>
       <c r="B44" s="22" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D44" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="E44" s="3" t="s">
         <v>140</v>
-      </c>
-      <c r="E44" s="3" t="s">
-        <v>141</v>
       </c>
       <c r="F44" s="3"/>
       <c r="G44" s="3"/>
@@ -3097,10 +3092,10 @@
         <v>81</v>
       </c>
       <c r="I44" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="J44" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="K44" s="6">
         <v>1.61</v>
@@ -3110,7 +3105,7 @@
         <v>1.61</v>
       </c>
       <c r="M44" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="N44" s="4" t="str">
         <f t="shared" si="1"/>
@@ -3121,15 +3116,15 @@
         <v>1x 512Kb EEPROM</v>
       </c>
     </row>
-    <row r="45" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15" ht="17" thickBot="1">
       <c r="A45" s="21">
         <v>3</v>
       </c>
       <c r="B45" s="16" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D45" s="3"/>
       <c r="E45" s="3"/>
@@ -3137,10 +3132,10 @@
       <c r="G45" s="3"/>
       <c r="H45" s="3"/>
       <c r="I45" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="J45" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="K45" s="6">
         <v>0.5</v>
@@ -3159,7 +3154,7 @@
         <v>3x IC Socket</v>
       </c>
     </row>
-    <row r="46" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15" ht="17" thickBot="1">
       <c r="A46" s="18"/>
       <c r="B46" s="4"/>
       <c r="C46" s="3"/>
@@ -3178,12 +3173,12 @@
         <v/>
       </c>
     </row>
-    <row r="47" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:15" ht="17" thickBot="1">
       <c r="A47" s="18">
         <v>0</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C47" s="3"/>
       <c r="D47" s="3"/>
@@ -3206,7 +3201,7 @@
         <v/>
       </c>
     </row>
-    <row r="48" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:15" ht="17" thickBot="1">
       <c r="A48" s="18"/>
       <c r="B48" s="4"/>
       <c r="C48" s="3"/>
@@ -3225,7 +3220,7 @@
         <v/>
       </c>
     </row>
-    <row r="49" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:14" ht="17" thickBot="1">
       <c r="A49" s="18"/>
       <c r="B49" s="4" t="s">
         <v>84</v>
@@ -3246,12 +3241,12 @@
         <v/>
       </c>
     </row>
-    <row r="50" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:14" ht="17" thickBot="1">
       <c r="A50" s="18">
         <v>1</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C50" s="3" t="s">
         <v>85</v>
@@ -3282,12 +3277,12 @@
         <v/>
       </c>
     </row>
-    <row r="51" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:14" ht="17" thickBot="1">
       <c r="A51" s="18">
         <v>1</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C51" s="3"/>
       <c r="D51" s="3"/>
@@ -3297,17 +3292,17 @@
       <c r="H51" s="3"/>
       <c r="I51" s="3"/>
       <c r="J51" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K51" s="3">
         <v>61.65</v>
       </c>
       <c r="L51" s="6"/>
       <c r="M51" s="4" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="52" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" ht="17" thickBot="1">
       <c r="A52" s="18"/>
       <c r="B52" s="4"/>
       <c r="C52" s="3"/>
@@ -3325,7 +3320,7 @@
       </c>
       <c r="L52" s="12">
         <f>SUM(L2:L51)</f>
-        <v>90.787999999999997</v>
+        <v>91.347999999999999</v>
       </c>
       <c r="M52" s="11" t="s">
         <v>83</v>
@@ -3353,6 +3348,11 @@
   <pageMargins left="0.75000000000000011" right="0.75000000000000011" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" scale="35" fitToHeight="2" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId13"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -3363,11 +3363,11 @@
   </sheetPr>
   <dimension ref="A1:O52"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8:K8"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="18.83203125" style="20" customWidth="1"/>
     <col min="2" max="2" width="46.6640625" customWidth="1"/>
@@ -3380,12 +3380,12 @@
     <col min="15" max="15" width="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="17" thickBot="1">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -3397,7 +3397,7 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>4</v>
@@ -3421,13 +3421,13 @@
         <v>10</v>
       </c>
       <c r="N1" s="23" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="O1" s="23" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="17" thickBot="1">
       <c r="A2" s="18"/>
       <c r="B2" s="4"/>
       <c r="C2" s="3"/>
@@ -3450,19 +3450,19 @@
         <v xml:space="preserve">x </v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" ht="17" thickBot="1">
       <c r="A3" s="21">
         <f>LEN(B3)-LEN(SUBSTITUTE(B3,",",""))+1</f>
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>12</v>
@@ -3475,10 +3475,10 @@
         <v>16</v>
       </c>
       <c r="I3" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="J3" s="2" t="s">
         <v>197</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>198</v>
       </c>
       <c r="K3" s="5">
         <v>1.7</v>
@@ -3497,19 +3497,19 @@
         <v>Capacitor - 1x 10uF</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" ht="17" thickBot="1">
       <c r="A4" s="21">
         <f>LEN(B4)-LEN(SUBSTITUTE(B4,",",""))+1</f>
         <v>5</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>15</v>
@@ -3522,10 +3522,10 @@
         <v>16</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="K4" s="5">
         <v>0.66</v>
@@ -3544,19 +3544,19 @@
         <v>Capacitor - 5x 0.22uF</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" ht="27" thickBot="1">
       <c r="A5" s="21">
         <f>LEN(B5)-LEN(SUBSTITUTE(B5,",",""))+1</f>
         <v>7</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>17</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>15</v>
@@ -3569,10 +3569,10 @@
         <v>16</v>
       </c>
       <c r="I5" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="J5" s="2" t="s">
         <v>191</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>192</v>
       </c>
       <c r="K5" s="5">
         <v>0.32</v>
@@ -3591,19 +3591,19 @@
         <v>Capacitor - 7x 0.1uF / 100nF</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" ht="17" thickBot="1">
       <c r="A6" s="21">
         <f>LEN(B6)-LEN(SUBSTITUTE(B6,",",""))+1</f>
         <v>1</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>18</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>12</v>
@@ -3616,10 +3616,10 @@
         <v>16</v>
       </c>
       <c r="I6" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="J6" s="2" t="s">
         <v>200</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>201</v>
       </c>
       <c r="K6" s="5">
         <v>1.57</v>
@@ -3638,19 +3638,19 @@
         <v>Capacitor - 1x 47uF</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" ht="27" thickBot="1">
       <c r="A7" s="21">
         <f t="shared" ref="A7:A9" si="3">LEN(B7)-LEN(SUBSTITUTE(B7,",",""))+1</f>
         <v>1</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>15</v>
@@ -3663,10 +3663,10 @@
         <v>13</v>
       </c>
       <c r="I7" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="J7" s="2" t="s">
         <v>202</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>203</v>
       </c>
       <c r="K7" s="5">
         <v>0.62</v>
@@ -3685,19 +3685,19 @@
         <v>Capacitor - 1x 0.33uF</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" ht="17" thickBot="1">
       <c r="A8" s="21">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>20</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>15</v>
@@ -3710,10 +3710,10 @@
         <v>16</v>
       </c>
       <c r="I8" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="J8" s="2" t="s">
         <v>206</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>207</v>
       </c>
       <c r="K8" s="5">
         <v>0.24</v>
@@ -3732,19 +3732,19 @@
         <v>Capacitor - 1x 0.01uF</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" ht="17" thickBot="1">
       <c r="A9" s="21">
         <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="B9" s="27" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>21</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>15</v>
@@ -3757,10 +3757,10 @@
         <v>16</v>
       </c>
       <c r="I9" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="J9" s="2" t="s">
         <v>188</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>189</v>
       </c>
       <c r="K9" s="5">
         <v>0.66</v>
@@ -3779,19 +3779,19 @@
         <v>Capacitor - 2x 1uF</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" ht="17" thickBot="1">
       <c r="A10" s="21">
         <f>LEN(B10)-LEN(SUBSTITUTE(B10,",",""))+1</f>
         <v>1</v>
       </c>
       <c r="B10" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>151</v>
-      </c>
       <c r="D10" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>15</v>
@@ -3802,10 +3802,10 @@
         <v>16</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K10" s="5">
         <v>0.25</v>
@@ -3824,7 +3824,7 @@
         <v>Capacitor - 1x 4.7nF</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" ht="17" thickBot="1">
       <c r="A11" s="18"/>
       <c r="B11" s="4"/>
       <c r="C11" s="3"/>
@@ -3843,7 +3843,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" ht="17" thickBot="1">
       <c r="A12" s="18"/>
       <c r="B12" s="4"/>
       <c r="C12" s="3"/>
@@ -3862,16 +3862,16 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="40" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" ht="40" thickBot="1">
       <c r="A13" s="21">
         <f>LEN(B13)-LEN(SUBSTITUTE(B13,",",""))+1</f>
         <v>1</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D13" s="7" t="s">
         <v>22</v>
@@ -3909,16 +3909,16 @@
         <v>Diode - 1x 1N5919BG Zener</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="40" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" ht="40" thickBot="1">
       <c r="A14" s="21">
         <f>LEN(B14)-LEN(SUBSTITUTE(B14,",",""))+1</f>
         <v>12</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>28</v>
@@ -3956,29 +3956,29 @@
         <v>Diode - 12x 1N5818-TP Schottky</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" ht="17" thickBot="1">
       <c r="A15" s="21">
         <f>LEN(B15)-LEN(SUBSTITUTE(B15,",",""))+1</f>
         <v>4</v>
       </c>
       <c r="B15" s="27" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>31</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
       <c r="J15" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K15" s="5">
         <v>0.47</v>
@@ -3997,13 +3997,13 @@
         <v>Diode - 4x LED-Red</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="40" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" ht="40" thickBot="1">
       <c r="A16" s="21">
         <f>LEN(B16)-LEN(SUBSTITUTE(B16,",",""))+1</f>
         <v>2</v>
       </c>
       <c r="B16" s="27" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>32</v>
@@ -4044,7 +4044,7 @@
         <v>Diode - 2x 1N4004</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" ht="17" thickBot="1">
       <c r="A17" s="18"/>
       <c r="B17" s="4"/>
       <c r="C17" s="3"/>
@@ -4067,7 +4067,7 @@
         <v xml:space="preserve">x </v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" ht="17" thickBot="1">
       <c r="A18" s="19"/>
       <c r="B18" s="4"/>
       <c r="C18" s="3"/>
@@ -4090,7 +4090,7 @@
         <v xml:space="preserve">x </v>
       </c>
     </row>
-    <row r="19" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" ht="17" thickBot="1">
       <c r="A19" s="18"/>
       <c r="B19" s="4"/>
       <c r="C19" s="3"/>
@@ -4113,12 +4113,12 @@
         <v xml:space="preserve">x </v>
       </c>
     </row>
-    <row r="20" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" ht="27" thickBot="1">
       <c r="A20" s="21">
         <v>1</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>36</v>
@@ -4159,7 +4159,7 @@
         <v>1x Surge Protection</v>
       </c>
     </row>
-    <row r="21" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" ht="17" thickBot="1">
       <c r="A21" s="18"/>
       <c r="B21" s="4"/>
       <c r="C21" s="3"/>
@@ -4182,30 +4182,30 @@
         <v xml:space="preserve">x </v>
       </c>
     </row>
-    <row r="22" spans="1:15" ht="40" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" ht="40" thickBot="1">
       <c r="A22" s="21">
         <v>14</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
       <c r="H22" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="K22" s="3">
         <v>0.40200000000000002</v>
@@ -4215,7 +4215,7 @@
         <v>5.6280000000000001</v>
       </c>
       <c r="M22" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="N22" s="4" t="str">
         <f t="shared" si="1"/>
@@ -4226,18 +4226,18 @@
         <v>14x Dual Terminal Block</v>
       </c>
     </row>
-    <row r="23" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" ht="17" thickBot="1">
       <c r="A23" s="21">
         <v>5</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>42</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
@@ -4245,7 +4245,7 @@
       <c r="H23" s="3"/>
       <c r="I23" s="3"/>
       <c r="J23" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="K23" s="5">
         <v>0.1</v>
@@ -4264,18 +4264,18 @@
         <v>5x Jumper</v>
       </c>
     </row>
-    <row r="24" spans="1:15" ht="40" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" ht="40" thickBot="1">
       <c r="A24" s="21">
         <v>1</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
@@ -4283,13 +4283,13 @@
         <v>1</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="K24" s="6">
         <v>0.56000000000000005</v>
@@ -4308,7 +4308,7 @@
         <v>1x 40 POS 0.100 Pin Header</v>
       </c>
     </row>
-    <row r="25" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" ht="17" thickBot="1">
       <c r="A25" s="18"/>
       <c r="B25" s="4"/>
       <c r="C25" s="3"/>
@@ -4331,7 +4331,7 @@
         <v xml:space="preserve">x </v>
       </c>
     </row>
-    <row r="26" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" ht="17" thickBot="1">
       <c r="A26" s="18"/>
       <c r="B26" s="4"/>
       <c r="C26" s="3"/>
@@ -4354,18 +4354,18 @@
         <v xml:space="preserve">x </v>
       </c>
     </row>
-    <row r="27" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" ht="27" thickBot="1">
       <c r="A27" s="21">
         <v>6</v>
       </c>
       <c r="B27" s="27" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>79</v>
@@ -4378,10 +4378,10 @@
         <v>43</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="K27" s="6">
         <v>1.51</v>
@@ -4400,7 +4400,7 @@
         <v>6x 62A MOSFET N-CH</v>
       </c>
     </row>
-    <row r="28" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" ht="17" thickBot="1">
       <c r="A28" s="18"/>
       <c r="B28" s="4"/>
       <c r="C28" s="3"/>
@@ -4419,7 +4419,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" ht="17" thickBot="1">
       <c r="A29" s="18"/>
       <c r="B29" s="4"/>
       <c r="C29" s="3"/>
@@ -4438,13 +4438,13 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" ht="17" thickBot="1">
       <c r="A30" s="21">
         <f>LEN(B30)-LEN(SUBSTITUTE(B30,",",""))+1</f>
         <v>5</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>44</v>
@@ -4483,13 +4483,13 @@
         <v>Resistor - 5x 10k</v>
       </c>
     </row>
-    <row r="31" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" ht="17" thickBot="1">
       <c r="A31" s="21">
         <f>LEN(B31)-LEN(SUBSTITUTE(B31,",",""))+1</f>
         <v>8</v>
       </c>
       <c r="B31" s="27" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>49</v>
@@ -4528,29 +4528,29 @@
         <v>Resistor - 8x 1k</v>
       </c>
     </row>
-    <row r="32" spans="1:15" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" ht="31" customHeight="1" thickBot="1">
       <c r="A32" s="21">
         <f>LEN(B32)-LEN(SUBSTITUTE(B32,",",""))+1</f>
         <v>4</v>
       </c>
       <c r="B32" s="28" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C32" s="14">
         <v>680</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E32" s="3"/>
       <c r="F32" s="14"/>
       <c r="G32" s="14"/>
       <c r="H32" s="14" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="I32" s="7"/>
       <c r="J32" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="K32" s="15">
         <v>0.22</v>
@@ -4560,7 +4560,7 @@
         <v>0.88</v>
       </c>
       <c r="M32" s="13" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="N32" s="4" t="str">
         <f t="shared" si="1"/>
@@ -4571,13 +4571,13 @@
         <v>Resistor - 4x 680</v>
       </c>
     </row>
-    <row r="33" spans="1:15" ht="40" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" ht="40" thickBot="1">
       <c r="A33" s="21">
         <f>LEN(B33)-LEN(SUBSTITUTE(B33,",",""))+1</f>
         <v>6</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>88</v>
+        <v>207</v>
       </c>
       <c r="C33" s="3">
         <v>470</v>
@@ -4616,16 +4616,16 @@
         <v>Resistor - 6x 470</v>
       </c>
     </row>
-    <row r="34" spans="1:15" ht="40" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" ht="40" thickBot="1">
       <c r="A34" s="21">
         <f>LEN(B34)-LEN(SUBSTITUTE(B34,",",""))+1</f>
         <v>2</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D34" s="3" t="s">
         <v>57</v>
@@ -4663,15 +4663,15 @@
         <v>Resistor - 2x 0.1% 2.49k</v>
       </c>
     </row>
-    <row r="35" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" ht="17" thickBot="1">
       <c r="A35" s="21">
         <v>1</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D35" s="3" t="s">
         <v>62</v>
@@ -4698,7 +4698,7 @@
         <v>0.46</v>
       </c>
       <c r="M35" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="N35" s="4" t="str">
         <f t="shared" si="1"/>
@@ -4709,15 +4709,15 @@
         <v>Resistor - 1x 0.1% 3.9k</v>
       </c>
     </row>
-    <row r="36" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" ht="17" thickBot="1">
       <c r="A36" s="21">
         <v>1</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D36" s="3" t="s">
         <v>65</v>
@@ -4744,7 +4744,7 @@
         <v>0.46</v>
       </c>
       <c r="M36" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="N36" s="4" t="str">
         <f t="shared" si="1"/>
@@ -4755,13 +4755,13 @@
         <v>Resistor - 1x 0.1% 1.0k</v>
       </c>
     </row>
-    <row r="37" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" ht="17" thickBot="1">
       <c r="A37" s="21">
         <f t="shared" ref="A37:A38" si="8">LEN(B37)-LEN(SUBSTITUTE(B37,",",""))+1</f>
         <v>8</v>
       </c>
       <c r="B37" s="27" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C37" s="3" t="s">
         <v>68</v>
@@ -4800,13 +4800,13 @@
         <v>Resistor - 8x 100k</v>
       </c>
     </row>
-    <row r="38" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" ht="17" thickBot="1">
       <c r="A38" s="21">
         <f t="shared" si="8"/>
         <v>2</v>
       </c>
       <c r="B38" s="27" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C38" s="3">
         <v>160</v>
@@ -4845,7 +4845,7 @@
         <v>Resistor - 2x 160</v>
       </c>
     </row>
-    <row r="39" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" ht="17" thickBot="1">
       <c r="A39" s="18"/>
       <c r="B39" s="4"/>
       <c r="C39" s="3"/>
@@ -4864,7 +4864,7 @@
         <v/>
       </c>
     </row>
-    <row r="40" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" ht="17" thickBot="1">
       <c r="A40" s="18"/>
       <c r="B40" s="4"/>
       <c r="C40" s="3"/>
@@ -4883,7 +4883,7 @@
         <v/>
       </c>
     </row>
-    <row r="41" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" ht="27" thickBot="1">
       <c r="A41" s="21">
         <v>1</v>
       </c>
@@ -4929,21 +4929,21 @@
         <v>1x LM2940T-5.0/NOPB</v>
       </c>
     </row>
-    <row r="42" spans="1:15" ht="40" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15" ht="40" thickBot="1">
       <c r="A42" s="21">
         <v>1</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F42" s="3"/>
       <c r="G42" s="3">
@@ -4954,7 +4954,7 @@
       </c>
       <c r="I42" s="3"/>
       <c r="J42" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K42" s="6">
         <v>15.41</v>
@@ -4973,21 +4973,21 @@
         <v>1x 1-Bar MAP sensor</v>
       </c>
     </row>
-    <row r="43" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" ht="27" thickBot="1">
       <c r="A43" s="21">
         <v>1</v>
       </c>
       <c r="B43" s="13" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C43" s="14" t="s">
+        <v>169</v>
+      </c>
+      <c r="D43" s="7" t="s">
         <v>170</v>
       </c>
-      <c r="D43" s="7" t="s">
+      <c r="E43" s="3" t="s">
         <v>171</v>
-      </c>
-      <c r="E43" s="3" t="s">
-        <v>172</v>
       </c>
       <c r="F43" s="14"/>
       <c r="G43" s="14">
@@ -4998,7 +4998,7 @@
       </c>
       <c r="I43" s="14"/>
       <c r="J43" s="14" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="K43" s="25">
         <v>2.92</v>
@@ -5017,21 +5017,21 @@
         <v>1x TC4424EPA</v>
       </c>
     </row>
-    <row r="44" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" ht="27" thickBot="1">
       <c r="A44" s="21">
         <v>1</v>
       </c>
       <c r="B44" s="22" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D44" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="E44" s="3" t="s">
         <v>140</v>
-      </c>
-      <c r="E44" s="3" t="s">
-        <v>141</v>
       </c>
       <c r="F44" s="3"/>
       <c r="G44" s="3"/>
@@ -5039,10 +5039,10 @@
         <v>81</v>
       </c>
       <c r="I44" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="J44" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="K44" s="6">
         <v>1.61</v>
@@ -5052,7 +5052,7 @@
         <v>1.61</v>
       </c>
       <c r="M44" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="N44" s="4" t="str">
         <f t="shared" si="1"/>
@@ -5063,15 +5063,15 @@
         <v>1x 512Kb EEPROM</v>
       </c>
     </row>
-    <row r="45" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15" ht="17" thickBot="1">
       <c r="A45" s="21">
         <v>3</v>
       </c>
       <c r="B45" s="16" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D45" s="3"/>
       <c r="E45" s="3"/>
@@ -5079,10 +5079,10 @@
       <c r="G45" s="3"/>
       <c r="H45" s="3"/>
       <c r="I45" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="J45" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="K45" s="6">
         <v>0.5</v>
@@ -5101,7 +5101,7 @@
         <v>3x IC Socket</v>
       </c>
     </row>
-    <row r="46" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15" ht="17" thickBot="1">
       <c r="A46" s="18"/>
       <c r="B46" s="4"/>
       <c r="C46" s="3"/>
@@ -5120,12 +5120,12 @@
         <v/>
       </c>
     </row>
-    <row r="47" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:15" ht="17" thickBot="1">
       <c r="A47" s="18">
         <v>0</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C47" s="3"/>
       <c r="D47" s="3"/>
@@ -5148,7 +5148,7 @@
         <v/>
       </c>
     </row>
-    <row r="48" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:15" ht="17" thickBot="1">
       <c r="A48" s="18"/>
       <c r="B48" s="4"/>
       <c r="C48" s="3"/>
@@ -5167,7 +5167,7 @@
         <v/>
       </c>
     </row>
-    <row r="49" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:14" ht="17" thickBot="1">
       <c r="A49" s="18"/>
       <c r="B49" s="4" t="s">
         <v>84</v>
@@ -5188,12 +5188,12 @@
         <v/>
       </c>
     </row>
-    <row r="50" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:14" ht="17" thickBot="1">
       <c r="A50" s="18">
         <v>1</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C50" s="3" t="s">
         <v>85</v>
@@ -5224,12 +5224,12 @@
         <v/>
       </c>
     </row>
-    <row r="51" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:14" ht="17" thickBot="1">
       <c r="A51" s="18">
         <v>1</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C51" s="3"/>
       <c r="D51" s="3"/>
@@ -5239,17 +5239,17 @@
       <c r="H51" s="3"/>
       <c r="I51" s="3"/>
       <c r="J51" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K51" s="3">
         <v>61.65</v>
       </c>
       <c r="L51" s="6"/>
       <c r="M51" s="4" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="52" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" ht="17" thickBot="1">
       <c r="A52" s="18"/>
       <c r="B52" s="4"/>
       <c r="C52" s="3"/>
@@ -5295,5 +5295,10 @@
   <pageMargins left="0.75000000000000011" right="0.75000000000000011" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" scale="35" fitToHeight="2" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId13"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Mix missing label in v0.3 BOM
</commit_message>
<xml_diff>
--- a/reference/hardware/v0.3/v0.3.1_bom.xlsx
+++ b/reference/hardware/v0.3/v0.3.1_bom.xlsx
@@ -1,16 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="25808"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/josh/Documents/Arduino/speeduino/speeduino/reference/hardware/v0.3/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16760" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Full Kit" sheetId="1" r:id="rId1"/>
     <sheet name="2 Channel" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -1416,11 +1421,11 @@
   </sheetPr>
   <dimension ref="A1:O52"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+    <sheetView topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.83203125" style="20" customWidth="1"/>
     <col min="2" max="2" width="46.6640625" customWidth="1"/>
@@ -1433,7 +1438,7 @@
     <col min="15" max="15" width="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="17" thickBot="1">
+    <row r="1" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
@@ -1480,7 +1485,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="17" thickBot="1">
+    <row r="2" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18"/>
       <c r="B2" s="4"/>
       <c r="C2" s="3"/>
@@ -1503,7 +1508,7 @@
         <v xml:space="preserve">x </v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="17" thickBot="1">
+    <row r="3" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="21">
         <f>LEN(B3)-LEN(SUBSTITUTE(B3,",",""))+1</f>
         <v>1</v>
@@ -1550,7 +1555,7 @@
         <v>Capacitor - 1x 10uF</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="17" thickBot="1">
+    <row r="4" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="21">
         <f>LEN(B4)-LEN(SUBSTITUTE(B4,",",""))+1</f>
         <v>5</v>
@@ -1597,7 +1602,7 @@
         <v>Capacitor - 5x 0.22uF</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="27" thickBot="1">
+    <row r="5" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="21">
         <f>LEN(B5)-LEN(SUBSTITUTE(B5,",",""))+1</f>
         <v>7</v>
@@ -1644,7 +1649,7 @@
         <v>Capacitor - 7x 0.1uF / 100nF</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="17" thickBot="1">
+    <row r="6" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="21">
         <f>LEN(B6)-LEN(SUBSTITUTE(B6,",",""))+1</f>
         <v>1</v>
@@ -1691,7 +1696,7 @@
         <v>Capacitor - 1x 47uF</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="27" thickBot="1">
+    <row r="7" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="21">
         <f t="shared" ref="A7:A9" si="3">LEN(B7)-LEN(SUBSTITUTE(B7,",",""))+1</f>
         <v>1</v>
@@ -1738,7 +1743,7 @@
         <v>Capacitor - 1x 0.33uF</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="17" thickBot="1">
+    <row r="8" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="21">
         <f t="shared" si="3"/>
         <v>1</v>
@@ -1785,7 +1790,7 @@
         <v>Capacitor - 1x 0.01uF</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="17" thickBot="1">
+    <row r="9" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="21">
         <f t="shared" si="3"/>
         <v>3</v>
@@ -1832,7 +1837,7 @@
         <v>Capacitor - 3x 1uF</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="17" thickBot="1">
+    <row r="10" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="21">
         <f>LEN(B10)-LEN(SUBSTITUTE(B10,",",""))+1</f>
         <v>1</v>
@@ -1877,7 +1882,7 @@
         <v>Capacitor - 1x 4.7nF</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="17" thickBot="1">
+    <row r="11" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="18"/>
       <c r="B11" s="4"/>
       <c r="C11" s="3"/>
@@ -1896,7 +1901,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="17" thickBot="1">
+    <row r="12" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="18"/>
       <c r="B12" s="4"/>
       <c r="C12" s="3"/>
@@ -1915,7 +1920,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="40" thickBot="1">
+    <row r="13" spans="1:15" ht="40" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="21">
         <f>LEN(B13)-LEN(SUBSTITUTE(B13,",",""))+1</f>
         <v>1</v>
@@ -1962,7 +1967,7 @@
         <v>Diode - 1x 1N5919BG Zener</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="40" thickBot="1">
+    <row r="14" spans="1:15" ht="40" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="21">
         <f>LEN(B14)-LEN(SUBSTITUTE(B14,",",""))+1</f>
         <v>12</v>
@@ -1993,11 +1998,11 @@
         <v>30</v>
       </c>
       <c r="K14" s="5">
-        <v>0.27</v>
+        <v>0.39</v>
       </c>
       <c r="L14" s="6">
         <f>K14*A14</f>
-        <v>3.24</v>
+        <v>4.68</v>
       </c>
       <c r="M14" s="4"/>
       <c r="N14" s="4" t="str">
@@ -2009,7 +2014,7 @@
         <v>Diode - 12x 1N5818-TP Schottky</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="17" thickBot="1">
+    <row r="15" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="21">
         <f>LEN(B15)-LEN(SUBSTITUTE(B15,",",""))+1</f>
         <v>8</v>
@@ -2050,7 +2055,7 @@
         <v>Diode - 8x LED-Red</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="40" thickBot="1">
+    <row r="16" spans="1:15" ht="40" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="21">
         <f>LEN(B16)-LEN(SUBSTITUTE(B16,",",""))+1</f>
         <v>4</v>
@@ -2097,7 +2102,7 @@
         <v>Diode - 4x 1N4004</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="17" thickBot="1">
+    <row r="17" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="18"/>
       <c r="B17" s="4"/>
       <c r="C17" s="3"/>
@@ -2120,7 +2125,7 @@
         <v xml:space="preserve">x </v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="17" thickBot="1">
+    <row r="18" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="19"/>
       <c r="B18" s="4"/>
       <c r="C18" s="3"/>
@@ -2143,7 +2148,7 @@
         <v xml:space="preserve">x </v>
       </c>
     </row>
-    <row r="19" spans="1:15" ht="17" thickBot="1">
+    <row r="19" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="18"/>
       <c r="B19" s="4"/>
       <c r="C19" s="3"/>
@@ -2166,7 +2171,7 @@
         <v xml:space="preserve">x </v>
       </c>
     </row>
-    <row r="20" spans="1:15" ht="27" thickBot="1">
+    <row r="20" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="21">
         <v>1</v>
       </c>
@@ -2212,7 +2217,7 @@
         <v>1x Surge Protection</v>
       </c>
     </row>
-    <row r="21" spans="1:15" ht="17" thickBot="1">
+    <row r="21" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="18"/>
       <c r="B21" s="4"/>
       <c r="C21" s="3"/>
@@ -2235,7 +2240,7 @@
         <v xml:space="preserve">x </v>
       </c>
     </row>
-    <row r="22" spans="1:15" ht="40" thickBot="1">
+    <row r="22" spans="1:15" ht="40" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="21">
         <v>14</v>
       </c>
@@ -2279,7 +2284,7 @@
         <v>14x Dual Terminal Block</v>
       </c>
     </row>
-    <row r="23" spans="1:15" ht="17" thickBot="1">
+    <row r="23" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="21">
         <v>5</v>
       </c>
@@ -2317,9 +2322,9 @@
         <v>5x Jumper</v>
       </c>
     </row>
-    <row r="24" spans="1:15" ht="40" thickBot="1">
+    <row r="24" spans="1:15" ht="40" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="21">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>119</v>
@@ -2349,19 +2354,19 @@
       </c>
       <c r="L24" s="6">
         <f>K24*A24</f>
-        <v>1.1200000000000001</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="M24" s="4"/>
       <c r="N24" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>2,S1012EC-40-ND</v>
+        <v>1,S1012EC-40-ND</v>
       </c>
       <c r="O24" t="str">
         <f t="shared" si="5"/>
-        <v>2x 40 POS 0.100 Pin Header</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" ht="17" thickBot="1">
+        <v>1x 40 POS 0.100 Pin Header</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="18"/>
       <c r="B25" s="4"/>
       <c r="C25" s="3"/>
@@ -2384,7 +2389,7 @@
         <v xml:space="preserve">x </v>
       </c>
     </row>
-    <row r="26" spans="1:15" ht="17" thickBot="1">
+    <row r="26" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="18"/>
       <c r="B26" s="4"/>
       <c r="C26" s="3"/>
@@ -2407,7 +2412,7 @@
         <v xml:space="preserve">x </v>
       </c>
     </row>
-    <row r="27" spans="1:15" ht="27" thickBot="1">
+    <row r="27" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="21">
         <f>LEN(B27)-LEN(SUBSTITUTE(B27,",",""))+1</f>
         <v>8</v>
@@ -2454,7 +2459,7 @@
         <v>8x 62A MOSFET N-CH</v>
       </c>
     </row>
-    <row r="28" spans="1:15" ht="17" thickBot="1">
+    <row r="28" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="18"/>
       <c r="B28" s="4"/>
       <c r="C28" s="3"/>
@@ -2473,7 +2478,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:15" ht="17" thickBot="1">
+    <row r="29" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="18"/>
       <c r="B29" s="4"/>
       <c r="C29" s="3"/>
@@ -2492,7 +2497,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:15" ht="17" thickBot="1">
+    <row r="30" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="21">
         <f>LEN(B30)-LEN(SUBSTITUTE(B30,",",""))+1</f>
         <v>5</v>
@@ -2537,7 +2542,7 @@
         <v>Resistor - 5x 10k</v>
       </c>
     </row>
-    <row r="31" spans="1:15" ht="17" thickBot="1">
+    <row r="31" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="21">
         <f>LEN(B31)-LEN(SUBSTITUTE(B31,",",""))+1</f>
         <v>12</v>
@@ -2582,7 +2587,7 @@
         <v>Resistor - 12x 1k</v>
       </c>
     </row>
-    <row r="32" spans="1:15" ht="27" thickBot="1">
+    <row r="32" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="21">
         <f>LEN(B32)-LEN(SUBSTITUTE(B32,",",""))+1</f>
         <v>8</v>
@@ -2625,7 +2630,7 @@
         <v>Resistor - 8x 680</v>
       </c>
     </row>
-    <row r="33" spans="1:15" ht="40" thickBot="1">
+    <row r="33" spans="1:15" ht="40" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="21">
         <f>LEN(B33)-LEN(SUBSTITUTE(B33,",",""))+1</f>
         <v>6</v>
@@ -2670,7 +2675,7 @@
         <v>Resistor - 6x 470</v>
       </c>
     </row>
-    <row r="34" spans="1:15" ht="40" thickBot="1">
+    <row r="34" spans="1:15" ht="40" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="21">
         <v>2</v>
       </c>
@@ -2716,7 +2721,7 @@
         <v>Resistor - 2x 0.1% 2.49k</v>
       </c>
     </row>
-    <row r="35" spans="1:15" ht="17" thickBot="1">
+    <row r="35" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="21">
         <v>1</v>
       </c>
@@ -2762,7 +2767,7 @@
         <v>Resistor - 1x 0.1% 3.9k</v>
       </c>
     </row>
-    <row r="36" spans="1:15" ht="17" thickBot="1">
+    <row r="36" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="21">
         <v>1</v>
       </c>
@@ -2808,7 +2813,7 @@
         <v>Resistor - 1x 0.1% 1.0k</v>
       </c>
     </row>
-    <row r="37" spans="1:15" ht="17" thickBot="1">
+    <row r="37" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="21">
         <f t="shared" ref="A37:A38" si="8">LEN(B37)-LEN(SUBSTITUTE(B37,",",""))+1</f>
         <v>12</v>
@@ -2853,7 +2858,7 @@
         <v>Resistor - 12x 100k</v>
       </c>
     </row>
-    <row r="38" spans="1:15" ht="17" thickBot="1">
+    <row r="38" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="21">
         <f t="shared" si="8"/>
         <v>4</v>
@@ -2898,7 +2903,7 @@
         <v>Resistor - 4x 160</v>
       </c>
     </row>
-    <row r="39" spans="1:15" ht="17" thickBot="1">
+    <row r="39" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="18"/>
       <c r="B39" s="4"/>
       <c r="C39" s="3"/>
@@ -2917,7 +2922,7 @@
         <v/>
       </c>
     </row>
-    <row r="40" spans="1:15" ht="17" thickBot="1">
+    <row r="40" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A40" s="18"/>
       <c r="B40" s="4"/>
       <c r="C40" s="3"/>
@@ -2936,7 +2941,7 @@
         <v/>
       </c>
     </row>
-    <row r="41" spans="1:15" ht="27" thickBot="1">
+    <row r="41" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="21">
         <v>1</v>
       </c>
@@ -2982,7 +2987,7 @@
         <v>1x LM2940T-5.0/NOPB</v>
       </c>
     </row>
-    <row r="42" spans="1:15" ht="40" thickBot="1">
+    <row r="42" spans="1:15" ht="40" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" s="21">
         <v>1</v>
       </c>
@@ -3026,7 +3031,7 @@
         <v>1x 1-Bar MAP sensor</v>
       </c>
     </row>
-    <row r="43" spans="1:15" ht="27" thickBot="1">
+    <row r="43" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A43" s="24">
         <v>2</v>
       </c>
@@ -3070,7 +3075,7 @@
         <v>2x TC4424EPA</v>
       </c>
     </row>
-    <row r="44" spans="1:15" ht="27" thickBot="1">
+    <row r="44" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A44" s="21">
         <v>1</v>
       </c>
@@ -3116,7 +3121,7 @@
         <v>1x 512Kb EEPROM</v>
       </c>
     </row>
-    <row r="45" spans="1:15" ht="17" thickBot="1">
+    <row r="45" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A45" s="21">
         <v>3</v>
       </c>
@@ -3154,7 +3159,7 @@
         <v>3x IC Socket</v>
       </c>
     </row>
-    <row r="46" spans="1:15" ht="17" thickBot="1">
+    <row r="46" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A46" s="18"/>
       <c r="B46" s="4"/>
       <c r="C46" s="3"/>
@@ -3173,7 +3178,7 @@
         <v/>
       </c>
     </row>
-    <row r="47" spans="1:15" ht="17" thickBot="1">
+    <row r="47" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A47" s="18">
         <v>0</v>
       </c>
@@ -3201,7 +3206,7 @@
         <v/>
       </c>
     </row>
-    <row r="48" spans="1:15" ht="17" thickBot="1">
+    <row r="48" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A48" s="18"/>
       <c r="B48" s="4"/>
       <c r="C48" s="3"/>
@@ -3220,7 +3225,7 @@
         <v/>
       </c>
     </row>
-    <row r="49" spans="1:14" ht="17" thickBot="1">
+    <row r="49" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A49" s="18"/>
       <c r="B49" s="4" t="s">
         <v>84</v>
@@ -3241,7 +3246,7 @@
         <v/>
       </c>
     </row>
-    <row r="50" spans="1:14" ht="17" thickBot="1">
+    <row r="50" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A50" s="18">
         <v>1</v>
       </c>
@@ -3277,7 +3282,7 @@
         <v/>
       </c>
     </row>
-    <row r="51" spans="1:14" ht="17" thickBot="1">
+    <row r="51" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A51" s="18">
         <v>1</v>
       </c>
@@ -3302,7 +3307,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="52" spans="1:14" ht="17" thickBot="1">
+    <row r="52" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A52" s="18"/>
       <c r="B52" s="4"/>
       <c r="C52" s="3"/>
@@ -3320,7 +3325,7 @@
       </c>
       <c r="L52" s="12">
         <f>SUM(L2:L51)</f>
-        <v>91.347999999999999</v>
+        <v>92.227999999999994</v>
       </c>
       <c r="M52" s="11" t="s">
         <v>83</v>
@@ -3348,11 +3353,6 @@
   <pageMargins left="0.75000000000000011" right="0.75000000000000011" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" scale="35" fitToHeight="2" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId13"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -3363,16 +3363,17 @@
   </sheetPr>
   <dimension ref="A1:O52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
       <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.83203125" style="20" customWidth="1"/>
     <col min="2" max="2" width="46.6640625" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
     <col min="4" max="4" width="53.1640625" customWidth="1"/>
+    <col min="7" max="7" width="0" hidden="1" customWidth="1"/>
     <col min="9" max="9" width="17.1640625" customWidth="1"/>
     <col min="10" max="10" width="28" customWidth="1"/>
     <col min="13" max="13" width="47.83203125" customWidth="1"/>
@@ -3380,7 +3381,7 @@
     <col min="15" max="15" width="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="17" thickBot="1">
+    <row r="1" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
@@ -3427,7 +3428,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="17" thickBot="1">
+    <row r="2" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18"/>
       <c r="B2" s="4"/>
       <c r="C2" s="3"/>
@@ -3450,7 +3451,7 @@
         <v xml:space="preserve">x </v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="17" thickBot="1">
+    <row r="3" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="21">
         <f>LEN(B3)-LEN(SUBSTITUTE(B3,",",""))+1</f>
         <v>1</v>
@@ -3497,7 +3498,7 @@
         <v>Capacitor - 1x 10uF</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="17" thickBot="1">
+    <row r="4" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="21">
         <f>LEN(B4)-LEN(SUBSTITUTE(B4,",",""))+1</f>
         <v>5</v>
@@ -3544,7 +3545,7 @@
         <v>Capacitor - 5x 0.22uF</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="27" thickBot="1">
+    <row r="5" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="21">
         <f>LEN(B5)-LEN(SUBSTITUTE(B5,",",""))+1</f>
         <v>7</v>
@@ -3591,7 +3592,7 @@
         <v>Capacitor - 7x 0.1uF / 100nF</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="17" thickBot="1">
+    <row r="6" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="21">
         <f>LEN(B6)-LEN(SUBSTITUTE(B6,",",""))+1</f>
         <v>1</v>
@@ -3638,7 +3639,7 @@
         <v>Capacitor - 1x 47uF</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="27" thickBot="1">
+    <row r="7" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="21">
         <f t="shared" ref="A7:A9" si="3">LEN(B7)-LEN(SUBSTITUTE(B7,",",""))+1</f>
         <v>1</v>
@@ -3685,7 +3686,7 @@
         <v>Capacitor - 1x 0.33uF</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="17" thickBot="1">
+    <row r="8" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="21">
         <f t="shared" si="3"/>
         <v>1</v>
@@ -3732,7 +3733,7 @@
         <v>Capacitor - 1x 0.01uF</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="17" thickBot="1">
+    <row r="9" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="21">
         <f t="shared" si="3"/>
         <v>2</v>
@@ -3779,7 +3780,7 @@
         <v>Capacitor - 2x 1uF</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="17" thickBot="1">
+    <row r="10" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="21">
         <f>LEN(B10)-LEN(SUBSTITUTE(B10,",",""))+1</f>
         <v>1</v>
@@ -3824,7 +3825,7 @@
         <v>Capacitor - 1x 4.7nF</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="17" thickBot="1">
+    <row r="11" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="18"/>
       <c r="B11" s="4"/>
       <c r="C11" s="3"/>
@@ -3843,7 +3844,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="17" thickBot="1">
+    <row r="12" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="18"/>
       <c r="B12" s="4"/>
       <c r="C12" s="3"/>
@@ -3862,7 +3863,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="40" thickBot="1">
+    <row r="13" spans="1:15" ht="40" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="21">
         <f>LEN(B13)-LEN(SUBSTITUTE(B13,",",""))+1</f>
         <v>1</v>
@@ -3909,7 +3910,7 @@
         <v>Diode - 1x 1N5919BG Zener</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="40" thickBot="1">
+    <row r="14" spans="1:15" ht="40" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="21">
         <f>LEN(B14)-LEN(SUBSTITUTE(B14,",",""))+1</f>
         <v>12</v>
@@ -3956,7 +3957,7 @@
         <v>Diode - 12x 1N5818-TP Schottky</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="17" thickBot="1">
+    <row r="15" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="21">
         <f>LEN(B15)-LEN(SUBSTITUTE(B15,",",""))+1</f>
         <v>4</v>
@@ -3997,7 +3998,7 @@
         <v>Diode - 4x LED-Red</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="40" thickBot="1">
+    <row r="16" spans="1:15" ht="40" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="21">
         <f>LEN(B16)-LEN(SUBSTITUTE(B16,",",""))+1</f>
         <v>2</v>
@@ -4044,7 +4045,7 @@
         <v>Diode - 2x 1N4004</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="17" thickBot="1">
+    <row r="17" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="18"/>
       <c r="B17" s="4"/>
       <c r="C17" s="3"/>
@@ -4067,7 +4068,7 @@
         <v xml:space="preserve">x </v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="17" thickBot="1">
+    <row r="18" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="19"/>
       <c r="B18" s="4"/>
       <c r="C18" s="3"/>
@@ -4090,7 +4091,7 @@
         <v xml:space="preserve">x </v>
       </c>
     </row>
-    <row r="19" spans="1:15" ht="17" thickBot="1">
+    <row r="19" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="18"/>
       <c r="B19" s="4"/>
       <c r="C19" s="3"/>
@@ -4113,7 +4114,7 @@
         <v xml:space="preserve">x </v>
       </c>
     </row>
-    <row r="20" spans="1:15" ht="27" thickBot="1">
+    <row r="20" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="21">
         <v>1</v>
       </c>
@@ -4159,7 +4160,7 @@
         <v>1x Surge Protection</v>
       </c>
     </row>
-    <row r="21" spans="1:15" ht="17" thickBot="1">
+    <row r="21" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="18"/>
       <c r="B21" s="4"/>
       <c r="C21" s="3"/>
@@ -4182,7 +4183,7 @@
         <v xml:space="preserve">x </v>
       </c>
     </row>
-    <row r="22" spans="1:15" ht="40" thickBot="1">
+    <row r="22" spans="1:15" ht="40" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="21">
         <v>14</v>
       </c>
@@ -4226,7 +4227,7 @@
         <v>14x Dual Terminal Block</v>
       </c>
     </row>
-    <row r="23" spans="1:15" ht="17" thickBot="1">
+    <row r="23" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="21">
         <v>5</v>
       </c>
@@ -4264,7 +4265,7 @@
         <v>5x Jumper</v>
       </c>
     </row>
-    <row r="24" spans="1:15" ht="40" thickBot="1">
+    <row r="24" spans="1:15" ht="40" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="21">
         <v>1</v>
       </c>
@@ -4308,7 +4309,7 @@
         <v>1x 40 POS 0.100 Pin Header</v>
       </c>
     </row>
-    <row r="25" spans="1:15" ht="17" thickBot="1">
+    <row r="25" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="18"/>
       <c r="B25" s="4"/>
       <c r="C25" s="3"/>
@@ -4331,7 +4332,7 @@
         <v xml:space="preserve">x </v>
       </c>
     </row>
-    <row r="26" spans="1:15" ht="17" thickBot="1">
+    <row r="26" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="18"/>
       <c r="B26" s="4"/>
       <c r="C26" s="3"/>
@@ -4354,7 +4355,7 @@
         <v xml:space="preserve">x </v>
       </c>
     </row>
-    <row r="27" spans="1:15" ht="27" thickBot="1">
+    <row r="27" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="21">
         <v>6</v>
       </c>
@@ -4400,7 +4401,7 @@
         <v>6x 62A MOSFET N-CH</v>
       </c>
     </row>
-    <row r="28" spans="1:15" ht="17" thickBot="1">
+    <row r="28" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="18"/>
       <c r="B28" s="4"/>
       <c r="C28" s="3"/>
@@ -4419,7 +4420,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:15" ht="17" thickBot="1">
+    <row r="29" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="18"/>
       <c r="B29" s="4"/>
       <c r="C29" s="3"/>
@@ -4438,7 +4439,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:15" ht="17" thickBot="1">
+    <row r="30" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="21">
         <f>LEN(B30)-LEN(SUBSTITUTE(B30,",",""))+1</f>
         <v>5</v>
@@ -4483,7 +4484,7 @@
         <v>Resistor - 5x 10k</v>
       </c>
     </row>
-    <row r="31" spans="1:15" ht="17" thickBot="1">
+    <row r="31" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="21">
         <f>LEN(B31)-LEN(SUBSTITUTE(B31,",",""))+1</f>
         <v>8</v>
@@ -4528,7 +4529,7 @@
         <v>Resistor - 8x 1k</v>
       </c>
     </row>
-    <row r="32" spans="1:15" ht="31" customHeight="1" thickBot="1">
+    <row r="32" spans="1:15" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="21">
         <f>LEN(B32)-LEN(SUBSTITUTE(B32,",",""))+1</f>
         <v>4</v>
@@ -4571,7 +4572,7 @@
         <v>Resistor - 4x 680</v>
       </c>
     </row>
-    <row r="33" spans="1:15" ht="40" thickBot="1">
+    <row r="33" spans="1:15" ht="40" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="21">
         <f>LEN(B33)-LEN(SUBSTITUTE(B33,",",""))+1</f>
         <v>6</v>
@@ -4616,7 +4617,7 @@
         <v>Resistor - 6x 470</v>
       </c>
     </row>
-    <row r="34" spans="1:15" ht="40" thickBot="1">
+    <row r="34" spans="1:15" ht="40" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="21">
         <f>LEN(B34)-LEN(SUBSTITUTE(B34,",",""))+1</f>
         <v>2</v>
@@ -4663,7 +4664,7 @@
         <v>Resistor - 2x 0.1% 2.49k</v>
       </c>
     </row>
-    <row r="35" spans="1:15" ht="17" thickBot="1">
+    <row r="35" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="21">
         <v>1</v>
       </c>
@@ -4709,7 +4710,7 @@
         <v>Resistor - 1x 0.1% 3.9k</v>
       </c>
     </row>
-    <row r="36" spans="1:15" ht="17" thickBot="1">
+    <row r="36" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="21">
         <v>1</v>
       </c>
@@ -4755,7 +4756,7 @@
         <v>Resistor - 1x 0.1% 1.0k</v>
       </c>
     </row>
-    <row r="37" spans="1:15" ht="17" thickBot="1">
+    <row r="37" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="21">
         <f t="shared" ref="A37:A38" si="8">LEN(B37)-LEN(SUBSTITUTE(B37,",",""))+1</f>
         <v>8</v>
@@ -4800,7 +4801,7 @@
         <v>Resistor - 8x 100k</v>
       </c>
     </row>
-    <row r="38" spans="1:15" ht="17" thickBot="1">
+    <row r="38" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="21">
         <f t="shared" si="8"/>
         <v>2</v>
@@ -4845,7 +4846,7 @@
         <v>Resistor - 2x 160</v>
       </c>
     </row>
-    <row r="39" spans="1:15" ht="17" thickBot="1">
+    <row r="39" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="18"/>
       <c r="B39" s="4"/>
       <c r="C39" s="3"/>
@@ -4864,7 +4865,7 @@
         <v/>
       </c>
     </row>
-    <row r="40" spans="1:15" ht="17" thickBot="1">
+    <row r="40" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A40" s="18"/>
       <c r="B40" s="4"/>
       <c r="C40" s="3"/>
@@ -4883,7 +4884,7 @@
         <v/>
       </c>
     </row>
-    <row r="41" spans="1:15" ht="27" thickBot="1">
+    <row r="41" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="21">
         <v>1</v>
       </c>
@@ -4929,7 +4930,7 @@
         <v>1x LM2940T-5.0/NOPB</v>
       </c>
     </row>
-    <row r="42" spans="1:15" ht="40" thickBot="1">
+    <row r="42" spans="1:15" ht="40" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" s="21">
         <v>1</v>
       </c>
@@ -4973,7 +4974,7 @@
         <v>1x 1-Bar MAP sensor</v>
       </c>
     </row>
-    <row r="43" spans="1:15" ht="27" thickBot="1">
+    <row r="43" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A43" s="21">
         <v>1</v>
       </c>
@@ -5017,7 +5018,7 @@
         <v>1x TC4424EPA</v>
       </c>
     </row>
-    <row r="44" spans="1:15" ht="27" thickBot="1">
+    <row r="44" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A44" s="21">
         <v>1</v>
       </c>
@@ -5063,7 +5064,7 @@
         <v>1x 512Kb EEPROM</v>
       </c>
     </row>
-    <row r="45" spans="1:15" ht="17" thickBot="1">
+    <row r="45" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A45" s="21">
         <v>3</v>
       </c>
@@ -5101,7 +5102,7 @@
         <v>3x IC Socket</v>
       </c>
     </row>
-    <row r="46" spans="1:15" ht="17" thickBot="1">
+    <row r="46" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A46" s="18"/>
       <c r="B46" s="4"/>
       <c r="C46" s="3"/>
@@ -5120,7 +5121,7 @@
         <v/>
       </c>
     </row>
-    <row r="47" spans="1:15" ht="17" thickBot="1">
+    <row r="47" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A47" s="18">
         <v>0</v>
       </c>
@@ -5148,7 +5149,7 @@
         <v/>
       </c>
     </row>
-    <row r="48" spans="1:15" ht="17" thickBot="1">
+    <row r="48" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A48" s="18"/>
       <c r="B48" s="4"/>
       <c r="C48" s="3"/>
@@ -5167,7 +5168,7 @@
         <v/>
       </c>
     </row>
-    <row r="49" spans="1:14" ht="17" thickBot="1">
+    <row r="49" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A49" s="18"/>
       <c r="B49" s="4" t="s">
         <v>84</v>
@@ -5188,7 +5189,7 @@
         <v/>
       </c>
     </row>
-    <row r="50" spans="1:14" ht="17" thickBot="1">
+    <row r="50" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A50" s="18">
         <v>1</v>
       </c>
@@ -5224,7 +5225,7 @@
         <v/>
       </c>
     </row>
-    <row r="51" spans="1:14" ht="17" thickBot="1">
+    <row r="51" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A51" s="18">
         <v>1</v>
       </c>
@@ -5249,7 +5250,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="52" spans="1:14" ht="17" thickBot="1">
+    <row r="52" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A52" s="18"/>
       <c r="B52" s="4"/>
       <c r="C52" s="3"/>
@@ -5295,10 +5296,5 @@
   <pageMargins left="0.75000000000000011" right="0.75000000000000011" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" scale="35" fitToHeight="2" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId13"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>